<commit_message>
Aktualisierung DoD und US
</commit_message>
<xml_diff>
--- a/Dokumente/UserStories_Kontaktsplitter_TeamSplitter.xlsx
+++ b/Dokumente/UserStories_Kontaktsplitter_TeamSplitter.xlsx
@@ -657,7 +657,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -735,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>25</v>

</xml_diff>